<commit_message>
SHAP Summary + new metrics
</commit_message>
<xml_diff>
--- a/results_morph/results_agg.xlsx
+++ b/results_morph/results_agg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stratifyenterprise.sharepoint.com/sites/StratifyInterno2/Shared Documents/Trendy/Maestros/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{C384D445-65B7-4DE2-97D0-0A29E4111283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85B2E163-97C6-4363-804F-B82CF87172DE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD33EC4-A691-49F0-BD93-CB4C9E471960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bin20" sheetId="1" r:id="rId1"/>
@@ -171,13 +171,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -425,9 +432,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -454,8 +461,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,23 +481,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,9 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -1083,60 +1105,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="34"/>
+      <c r="L1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="22"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="19" t="s">
         <v>24</v>
       </c>
@@ -1198,7 +1220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1253,7 +1275,7 @@
       <c r="V3" s="11"/>
       <c r="W3" s="12"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1330,7 @@
       <c r="V4" s="4"/>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1385,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1440,7 @@
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>1</v>
       </c>
@@ -1473,7 +1495,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="18"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1528,7 +1550,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1605,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1660,7 @@
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
@@ -1693,7 +1715,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="18"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1770,7 @@
       <c r="V12" s="4"/>
       <c r="W12" s="5"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1803,7 +1825,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>1</v>
       </c>
@@ -1871,25 +1893,25 @@
       <c r="D15" s="17">
         <v>0.52654387865655472</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="25">
         <v>0.70422535211267601</v>
       </c>
       <c r="F15" s="17">
         <v>0.17145178764897076</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="25">
         <v>0.12567713976164679</v>
       </c>
       <c r="H15" s="17">
         <v>0.6819170221755142</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="25">
         <v>0.70783729051422362</v>
       </c>
       <c r="J15" s="17">
         <v>0.83023747199306108</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="25">
         <v>0.86294054517382379</v>
       </c>
       <c r="L15" s="17">
@@ -2142,7 +2164,7 @@
         <v>0.21194543128133339</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>1</v>
       </c>
@@ -2197,7 +2219,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="18"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2252,7 +2274,7 @@
       <c r="V20" s="4"/>
       <c r="W20" s="5"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2307,7 +2329,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>1</v>
       </c>
@@ -2362,7 +2384,7 @@
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2439,7 @@
       <c r="V23" s="11"/>
       <c r="W23" s="12"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -2472,7 +2494,7 @@
       <c r="V24" s="4"/>
       <c r="W24" s="5"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2527,7 +2549,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="5"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>2</v>
       </c>
@@ -2582,7 +2604,7 @@
       <c r="V26" s="14"/>
       <c r="W26" s="15"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2659,7 @@
       <c r="V27" s="17"/>
       <c r="W27" s="18"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -2692,7 +2714,7 @@
       <c r="V28" s="4"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -2747,7 +2769,7 @@
       <c r="V29" s="4"/>
       <c r="W29" s="5"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
@@ -2802,7 +2824,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="15"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>2</v>
       </c>
@@ -2857,7 +2879,7 @@
       <c r="V31" s="17"/>
       <c r="W31" s="18"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -2912,7 +2934,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="5"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -2967,7 +2989,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="5"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3044,7 @@
       <c r="V34" s="14"/>
       <c r="W34" s="15"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>2</v>
       </c>
@@ -3077,7 +3099,7 @@
       <c r="V35" s="17"/>
       <c r="W35" s="18"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -3132,7 +3154,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="5"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -3187,7 +3209,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="5"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>2</v>
       </c>
@@ -3255,13 +3277,13 @@
       <c r="D39" s="17">
         <v>0.78597122302158273</v>
       </c>
-      <c r="E39" s="31">
+      <c r="E39" s="25">
         <v>0.8039568345323741</v>
       </c>
-      <c r="F39" s="32">
+      <c r="F39" s="26">
         <v>7.1942446043165464E-2</v>
       </c>
-      <c r="G39" s="28">
+      <c r="G39" s="22">
         <v>7.2392086330935246E-2</v>
       </c>
       <c r="H39" s="17">
@@ -3400,19 +3422,19 @@
       <c r="E41" s="5">
         <v>0.80215827338129497</v>
       </c>
-      <c r="F41" s="33">
+      <c r="F41" s="27">
         <v>7.2392086330935246E-2</v>
       </c>
       <c r="G41" s="5">
         <v>7.4190647482014385E-2</v>
       </c>
-      <c r="H41" s="33">
+      <c r="H41" s="27">
         <v>0.6668972927488972</v>
       </c>
       <c r="I41" s="5">
         <v>0.60327857769953452</v>
       </c>
-      <c r="J41" s="33">
+      <c r="J41" s="27">
         <v>0.91990056408269494</v>
       </c>
       <c r="K41" s="5">
@@ -3468,7 +3490,7 @@
       <c r="D42" s="6">
         <v>0.79136690647482011</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="28">
         <v>0.8039568345323741</v>
       </c>
       <c r="F42" s="6">
@@ -3526,7 +3548,7 @@
         <v>0.23287193828680897</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>3</v>
       </c>
@@ -3581,7 +3603,7 @@
       <c r="V43" s="11"/>
       <c r="W43" s="12"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -3636,7 +3658,7 @@
       <c r="V44" s="4"/>
       <c r="W44" s="5"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3691,7 +3713,7 @@
       <c r="V45" s="4"/>
       <c r="W45" s="5"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>3</v>
       </c>
@@ -3746,7 +3768,7 @@
       <c r="V46" s="14"/>
       <c r="W46" s="15"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>3</v>
       </c>
@@ -3801,7 +3823,7 @@
       <c r="V47" s="17"/>
       <c r="W47" s="18"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -3856,7 +3878,7 @@
       <c r="V48" s="4"/>
       <c r="W48" s="5"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -3911,7 +3933,7 @@
       <c r="V49" s="4"/>
       <c r="W49" s="5"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>3</v>
       </c>
@@ -3966,7 +3988,7 @@
       <c r="V50" s="14"/>
       <c r="W50" s="15"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>3</v>
       </c>
@@ -4021,7 +4043,7 @@
       <c r="V51" s="17"/>
       <c r="W51" s="18"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -4076,7 +4098,7 @@
       <c r="V52" s="4"/>
       <c r="W52" s="5"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -4131,7 +4153,7 @@
       <c r="V53" s="4"/>
       <c r="W53" s="5"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>3</v>
       </c>
@@ -4205,10 +4227,10 @@
       <c r="F55" s="17">
         <v>0.12872023809523808</v>
       </c>
-      <c r="G55" s="29">
+      <c r="G55" s="23">
         <v>0.12053571428571429</v>
       </c>
-      <c r="H55" s="32">
+      <c r="H55" s="26">
         <v>0.61189529929271202</v>
       </c>
       <c r="I55" s="18">
@@ -4217,7 +4239,7 @@
       <c r="J55" s="17">
         <v>0.8543142828485677</v>
       </c>
-      <c r="K55" s="31">
+      <c r="K55" s="25">
         <v>0.85802438344684717</v>
       </c>
       <c r="L55" s="17">
@@ -4270,13 +4292,13 @@
       <c r="D56" s="4">
         <v>0.7857142857142857</v>
       </c>
-      <c r="E56" s="35">
+      <c r="E56" s="29">
         <v>0.8102678571428571</v>
       </c>
       <c r="F56" s="4">
         <v>0.12351190476190477</v>
       </c>
-      <c r="G56" s="35">
+      <c r="G56" s="29">
         <v>0.11532738095238096</v>
       </c>
       <c r="H56" s="4">
@@ -4347,7 +4369,7 @@
       <c r="F57" s="4">
         <v>0.12797619047619047</v>
       </c>
-      <c r="G57" s="30">
+      <c r="G57" s="24">
         <v>0.11830357142857142</v>
       </c>
       <c r="H57" s="4">
@@ -4412,7 +4434,7 @@
       <c r="D58" s="6">
         <v>0.7879464285714286</v>
       </c>
-      <c r="E58" s="34">
+      <c r="E58" s="28">
         <v>0.8102678571428571</v>
       </c>
       <c r="F58" s="6">
@@ -4470,7 +4492,7 @@
         <v>5.823372760600401E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
@@ -4525,7 +4547,7 @@
       <c r="V59" s="11"/>
       <c r="W59" s="12"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -4580,7 +4602,7 @@
       <c r="V60" s="4"/>
       <c r="W60" s="5"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -4635,7 +4657,7 @@
       <c r="V61" s="4"/>
       <c r="W61" s="5"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>4</v>
       </c>
@@ -4690,7 +4712,7 @@
       <c r="V62" s="14"/>
       <c r="W62" s="15"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>4</v>
       </c>
@@ -4745,7 +4767,7 @@
       <c r="V63" s="17"/>
       <c r="W63" s="18"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -4800,7 +4822,7 @@
       <c r="V64" s="4"/>
       <c r="W64" s="5"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -4855,7 +4877,7 @@
       <c r="V65" s="4"/>
       <c r="W65" s="5"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>4</v>
       </c>
@@ -4923,22 +4945,22 @@
       <c r="D67" s="17">
         <v>0.7482319660537482</v>
       </c>
-      <c r="E67" s="31">
+      <c r="E67" s="25">
         <v>0.74964639321074966</v>
       </c>
-      <c r="F67" s="32">
+      <c r="F67" s="26">
         <v>9.8066949552098062E-2</v>
       </c>
       <c r="G67" s="18">
         <v>0.10278170674210278</v>
       </c>
-      <c r="H67" s="32">
+      <c r="H67" s="26">
         <v>0.71246638203945378</v>
       </c>
       <c r="I67" s="18">
         <v>0.68271181886986942</v>
       </c>
-      <c r="J67" s="32">
+      <c r="J67" s="26">
         <v>0.89319320942299463</v>
       </c>
       <c r="K67" s="18">
@@ -5065,7 +5087,7 @@
       <c r="D69" s="4">
         <v>0.73974540311173975</v>
       </c>
-      <c r="E69" s="30">
+      <c r="E69" s="24">
         <v>0.74540311173974538</v>
       </c>
       <c r="F69" s="4">
@@ -5194,7 +5216,7 @@
         <v>0.21608338546670575</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>4</v>
       </c>
@@ -5249,7 +5271,7 @@
       <c r="V71" s="17"/>
       <c r="W71" s="18"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -5304,7 +5326,7 @@
       <c r="V72" s="4"/>
       <c r="W72" s="5"/>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -5359,7 +5381,7 @@
       <c r="V73" s="4"/>
       <c r="W73" s="5"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>4</v>
       </c>
@@ -5415,7 +5437,7 @@
       <c r="W74" s="7"/>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C76" s="36" t="s">
+      <c r="C76" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D76" s="2" cm="1">
@@ -5500,13 +5522,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:C74" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Overall"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="13">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="H1:I1"/>
@@ -5515,6 +5538,11 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D74">
     <cfRule type="expression" dxfId="39" priority="23">
@@ -5623,10 +5651,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F08E22B-B94A-4313-AA71-C1A31F770FAE}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5637,60 +5666,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="34"/>
+      <c r="L1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="22"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="19" t="s">
         <v>24</v>
       </c>
@@ -5752,7 +5781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5762,19 +5791,27 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12">
+      <c r="D3" s="43">
+        <v>0.89057421451787644</v>
+      </c>
+      <c r="E3" s="42">
         <v>0.89165763813651133</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12">
+      <c r="F3" s="43">
+        <v>0.10942578548212351</v>
+      </c>
+      <c r="G3" s="42">
         <v>0.10834236186348863</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="H3" s="11">
+        <v>0.77887915596321577</v>
+      </c>
       <c r="I3" s="12">
         <v>0.79072572599807733</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="11">
+        <v>0.88359327335821025</v>
+      </c>
       <c r="K3" s="12">
         <v>0.88756367602169195</v>
       </c>
@@ -5782,11 +5819,15 @@
       <c r="M3" s="12"/>
       <c r="N3" s="11"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="11">
+        <v>0.665424430641822</v>
+      </c>
       <c r="Q3" s="12">
         <v>0.67812374144180421</v>
       </c>
-      <c r="R3" s="11"/>
+      <c r="R3" s="11">
+        <v>0.80823867396127047</v>
+      </c>
       <c r="S3" s="12">
         <v>0.81250687230044039</v>
       </c>
@@ -5795,7 +5836,7 @@
       <c r="V3" s="11"/>
       <c r="W3" s="12"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5805,16 +5846,16 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="44">
         <v>0.84398699891657636</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="45">
         <v>0.83206933911159264</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="44">
         <v>0.15601300108342361</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="45">
         <v>0.16793066088840736</v>
       </c>
       <c r="H4" s="4">
@@ -5850,7 +5891,7 @@
       <c r="V4" s="4"/>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5860,16 +5901,16 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="44">
         <v>0.89274106175514623</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="45">
         <v>0.88840736728060676</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="44">
         <v>0.10725893824485373</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="45">
         <v>0.11159263271939328</v>
       </c>
       <c r="H5" s="4">
@@ -5905,7 +5946,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -5915,16 +5956,16 @@
       <c r="C6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="46">
         <v>0.8819068255687974</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="47">
         <v>0.87648970747562294</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="46">
         <v>0.1180931744312026</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="47">
         <v>0.12351029252437704</v>
       </c>
       <c r="H6" s="14">
@@ -5960,7 +6001,7 @@
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>1</v>
       </c>
@@ -5970,19 +6011,27 @@
       <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18">
+      <c r="D7" s="41">
+        <v>0.88949079089924166</v>
+      </c>
+      <c r="E7" s="48">
         <v>0.88840736728060676</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18">
+      <c r="F7" s="41">
+        <v>0.1105092091007584</v>
+      </c>
+      <c r="G7" s="48">
         <v>0.11159263271939328</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="17">
+        <v>0.81443945127719974</v>
+      </c>
       <c r="I7" s="18">
         <v>0.81475433793513319</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17">
+        <v>0.88437655991988617</v>
+      </c>
       <c r="K7" s="18">
         <v>0.88397806139213331</v>
       </c>
@@ -5990,11 +6039,15 @@
       <c r="M7" s="18"/>
       <c r="N7" s="17"/>
       <c r="O7" s="18"/>
-      <c r="P7" s="17"/>
+      <c r="P7" s="17">
+        <v>0.70384785342805678</v>
+      </c>
       <c r="Q7" s="18">
         <v>0.70396329164985882</v>
       </c>
-      <c r="R7" s="17"/>
+      <c r="R7" s="17">
+        <v>0.80435912007249688</v>
+      </c>
       <c r="S7" s="18">
         <v>0.80348247780452942</v>
       </c>
@@ -6003,7 +6056,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="18"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -6013,16 +6066,16 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="44">
         <v>0.80498374864572053</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="45">
         <v>0.79739978331527628</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="44">
         <v>0.19501625135427952</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="45">
         <v>0.20260021668472372</v>
       </c>
       <c r="H8" s="4">
@@ -6058,7 +6111,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -6068,16 +6121,16 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="44">
         <v>0.87648970747562294</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="45">
         <v>0.87757313109425783</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="44">
         <v>0.12351029252437704</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="45">
         <v>0.12242686890574214</v>
       </c>
       <c r="H9" s="4">
@@ -6113,7 +6166,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>1</v>
       </c>
@@ -6123,16 +6176,16 @@
       <c r="C10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="46">
         <v>0.86132177681473454</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="47">
         <v>0.85157096424702061</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="46">
         <v>0.13867822318526543</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="47">
         <v>0.14842903575297942</v>
       </c>
       <c r="H10" s="14">
@@ -6168,7 +6221,7 @@
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
@@ -6178,19 +6231,27 @@
       <c r="C11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18">
+      <c r="D11" s="41">
+        <v>0.78764897074756235</v>
+      </c>
+      <c r="E11" s="48">
         <v>0.78548212351029256</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18">
+      <c r="F11" s="41">
+        <v>0.21235102925243771</v>
+      </c>
+      <c r="G11" s="48">
         <v>0.21451787648970747</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="17">
+        <v>0.73253022023513825</v>
+      </c>
       <c r="I11" s="18">
         <v>0.72566379651979673</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="17">
+        <v>0.78422871415251938</v>
+      </c>
       <c r="K11" s="18">
         <v>0.78020811788236022</v>
       </c>
@@ -6198,11 +6259,15 @@
       <c r="M11" s="18"/>
       <c r="N11" s="17"/>
       <c r="O11" s="18"/>
-      <c r="P11" s="17"/>
+      <c r="P11" s="17">
+        <v>0.5925617685305592</v>
+      </c>
       <c r="Q11" s="18">
         <v>0.5854661586732407</v>
       </c>
-      <c r="R11" s="17"/>
+      <c r="R11" s="17">
+        <v>0.65752035469795866</v>
+      </c>
       <c r="S11" s="18">
         <v>0.65332750910177817</v>
       </c>
@@ -6211,7 +6276,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="18"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -6221,16 +6286,16 @@
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="44">
         <v>0.6912242686890574</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="45">
         <v>0.70747562296858069</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="44">
         <v>0.3087757313109426</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="45">
         <v>0.29252437703141926</v>
       </c>
       <c r="H12" s="4">
@@ -6266,7 +6331,7 @@
       <c r="V12" s="4"/>
       <c r="W12" s="5"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -6276,16 +6341,16 @@
       <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="44">
         <v>0.79631635969664138</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="45">
         <v>0.8082340195016251</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="44">
         <v>0.20368364030335862</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="45">
         <v>0.19176598049837487</v>
       </c>
       <c r="H13" s="4">
@@ -6321,7 +6386,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>1</v>
       </c>
@@ -6331,16 +6396,16 @@
       <c r="C14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="46">
         <v>0.77573131094257852</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="47">
         <v>0.77789815817984831</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="46">
         <v>0.22426868905742145</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="47">
         <v>0.22210184182015169</v>
       </c>
       <c r="H14" s="14">
@@ -6386,43 +6451,63 @@
       <c r="C15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="17">
+        <v>0.65330444203683635</v>
+      </c>
       <c r="E15" s="18">
         <v>0.67930660888407368</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="17">
+        <v>0.12594799566630552</v>
+      </c>
       <c r="G15" s="18">
         <v>0.12757313109425786</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18">
+      <c r="H15" s="17">
+        <v>0.72617558002302807</v>
+      </c>
+      <c r="I15" s="22">
         <v>0.73664013177991849</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18">
+      <c r="J15" s="17">
+        <v>0.86559996518336624</v>
+      </c>
+      <c r="K15" s="22">
         <v>0.86617757758352631</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="17">
+        <v>0.53109612005028561</v>
+      </c>
       <c r="M15" s="18">
         <v>0.55293289848533034</v>
       </c>
-      <c r="N15" s="17"/>
+      <c r="N15" s="17">
+        <v>0.59837465246553001</v>
+      </c>
       <c r="O15" s="18">
         <v>0.60600045627597832</v>
       </c>
-      <c r="P15" s="17"/>
+      <c r="P15" s="17">
+        <v>0.619955633221</v>
+      </c>
       <c r="Q15" s="18">
         <v>0.62685122657885328</v>
       </c>
-      <c r="R15" s="17"/>
+      <c r="R15" s="17">
+        <v>0.78550841690274875</v>
+      </c>
       <c r="S15" s="18">
         <v>0.78501979544244327</v>
       </c>
-      <c r="T15" s="17"/>
+      <c r="T15" s="17">
+        <v>0.3833604099930783</v>
+      </c>
       <c r="U15" s="18">
         <v>0.39879732228944698</v>
       </c>
-      <c r="V15" s="17"/>
+      <c r="V15" s="17">
+        <v>0.43778590787991378</v>
+      </c>
       <c r="W15" s="18">
         <v>0.44317465056902211</v>
       </c>
@@ -6511,13 +6596,13 @@
       <c r="D17" s="4">
         <v>0.6619718309859155</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="39">
         <v>0.70747562296858069</v>
       </c>
       <c r="F17" s="4">
         <v>0.12567713976164679</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="39">
         <v>0.12405200433369447</v>
       </c>
       <c r="H17" s="4">
@@ -6640,7 +6725,7 @@
         <v>0.28923936363644892</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>1</v>
       </c>
@@ -6650,19 +6735,27 @@
       <c r="C19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18">
+      <c r="D19" s="41">
+        <v>0.92849404117009748</v>
+      </c>
+      <c r="E19" s="48">
         <v>0.92416034669555791</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18">
+      <c r="F19" s="41">
+        <v>7.1505958829902488E-2</v>
+      </c>
+      <c r="G19" s="48">
         <v>7.5839653304442034E-2</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="17">
+        <v>0.57885349261655883</v>
+      </c>
       <c r="I19" s="18">
         <v>0.61541666666666661</v>
       </c>
-      <c r="J19" s="17"/>
+      <c r="J19" s="17">
+        <v>0.91020131330284926</v>
+      </c>
       <c r="K19" s="18">
         <v>0.91296045503791978</v>
       </c>
@@ -6670,11 +6763,15 @@
       <c r="M19" s="18"/>
       <c r="N19" s="17"/>
       <c r="O19" s="18"/>
-      <c r="P19" s="17"/>
+      <c r="P19" s="17">
+        <v>0.51798848028356226</v>
+      </c>
       <c r="Q19" s="18">
         <v>0.53985171455050973</v>
       </c>
-      <c r="R19" s="17"/>
+      <c r="R19" s="17">
+        <v>0.87191551887926866</v>
+      </c>
       <c r="S19" s="18">
         <v>0.87076232256302499</v>
       </c>
@@ -6683,7 +6780,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="18"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -6693,16 +6790,16 @@
       <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="44">
         <v>0.93174431202600216</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="45">
         <v>0.93174431202600216</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="44">
         <v>6.8255687973997836E-2</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="45">
         <v>6.8255687973997836E-2</v>
       </c>
       <c r="H20" s="4">
@@ -6738,7 +6835,7 @@
       <c r="V20" s="4"/>
       <c r="W20" s="5"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -6748,16 +6845,16 @@
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="44">
         <v>0.93174431202600216</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="45">
         <v>0.92957746478873238</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="44">
         <v>6.8255687973997836E-2</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="45">
         <v>7.0422535211267609E-2</v>
       </c>
       <c r="H21" s="4">
@@ -6793,7 +6890,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>1</v>
       </c>
@@ -6803,16 +6900,16 @@
       <c r="C22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="49">
         <v>0.93499458288190684</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="50">
         <v>0.9252437703141928</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="49">
         <v>6.500541711809317E-2</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="50">
         <v>7.4756229685807155E-2</v>
       </c>
       <c r="H22" s="6">
@@ -6848,7 +6945,7 @@
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
@@ -6858,19 +6955,27 @@
       <c r="C23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12">
+      <c r="D23" s="43">
+        <v>0.90827338129496404</v>
+      </c>
+      <c r="E23" s="42">
         <v>0.89388489208633093</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12">
+      <c r="F23" s="43">
+        <v>9.172661870503597E-2</v>
+      </c>
+      <c r="G23" s="42">
         <v>0.10611510791366907</v>
       </c>
-      <c r="H23" s="11"/>
+      <c r="H23" s="11">
+        <v>0.77934962765833271</v>
+      </c>
       <c r="I23" s="12">
         <v>0.7632625372563453</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="11">
+        <v>0.8994762310468174</v>
+      </c>
       <c r="K23" s="12">
         <v>0.88850818498679152</v>
       </c>
@@ -6878,11 +6983,15 @@
       <c r="M23" s="12"/>
       <c r="N23" s="11"/>
       <c r="O23" s="12"/>
-      <c r="P23" s="11"/>
+      <c r="P23" s="11">
+        <v>0.67036161512905701</v>
+      </c>
       <c r="Q23" s="12">
         <v>0.65052779597025845</v>
       </c>
-      <c r="R23" s="11"/>
+      <c r="R23" s="11">
+        <v>0.83474518621749672</v>
+      </c>
       <c r="S23" s="12">
         <v>0.81767840726070762</v>
       </c>
@@ -6891,7 +7000,7 @@
       <c r="V23" s="11"/>
       <c r="W23" s="12"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -6901,16 +7010,16 @@
       <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="44">
         <v>0.88669064748201443</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="45">
         <v>0.87410071942446044</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="44">
         <v>0.11330935251798561</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="45">
         <v>0.12589928057553956</v>
       </c>
       <c r="H24" s="4">
@@ -6946,7 +7055,7 @@
       <c r="V24" s="4"/>
       <c r="W24" s="5"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -6956,16 +7065,16 @@
       <c r="C25" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="44">
         <v>0.89928057553956831</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="45">
         <v>0.90287769784172667</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="44">
         <v>0.10071942446043165</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="45">
         <v>9.7122302158273388E-2</v>
       </c>
       <c r="H25" s="4">
@@ -7001,7 +7110,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="5"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>2</v>
       </c>
@@ -7011,16 +7120,16 @@
       <c r="C26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="46">
         <v>0.87589928057553956</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="47">
         <v>0.89748201438848918</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="46">
         <v>0.12410071942446044</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="47">
         <v>0.10251798561151079</v>
       </c>
       <c r="H26" s="14">
@@ -7056,7 +7165,7 @@
       <c r="V26" s="14"/>
       <c r="W26" s="15"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>2</v>
       </c>
@@ -7066,19 +7175,27 @@
       <c r="C27" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18">
+      <c r="D27" s="41">
+        <v>0.83273381294964033</v>
+      </c>
+      <c r="E27" s="48">
         <v>0.82913669064748197</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18">
+      <c r="F27" s="41">
+        <v>0.1672661870503597</v>
+      </c>
+      <c r="G27" s="48">
         <v>0.17086330935251798</v>
       </c>
-      <c r="H27" s="17"/>
+      <c r="H27" s="17">
+        <v>0.71313971873179671</v>
+      </c>
       <c r="I27" s="18">
         <v>0.67484779651209315</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="17">
+        <v>0.83173441940464443</v>
+      </c>
       <c r="K27" s="18">
         <v>0.81825992787553548</v>
       </c>
@@ -7086,11 +7203,15 @@
       <c r="M27" s="18"/>
       <c r="N27" s="17"/>
       <c r="O27" s="18"/>
-      <c r="P27" s="17"/>
+      <c r="P27" s="17">
+        <v>0.58704844006568146</v>
+      </c>
       <c r="Q27" s="18">
         <v>0.55364617916221603</v>
       </c>
-      <c r="R27" s="17"/>
+      <c r="R27" s="17">
+        <v>0.73330793493284185</v>
+      </c>
       <c r="S27" s="18">
         <v>0.72178664585869345</v>
       </c>
@@ -7099,7 +7220,7 @@
       <c r="V27" s="17"/>
       <c r="W27" s="18"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -7109,16 +7230,16 @@
       <c r="C28" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="44">
         <v>0.82374100719424459</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="45">
         <v>0.82194244604316546</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="44">
         <v>0.17625899280575538</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="45">
         <v>0.17805755395683454</v>
       </c>
       <c r="H28" s="4">
@@ -7154,7 +7275,7 @@
       <c r="V28" s="4"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -7164,16 +7285,16 @@
       <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="44">
         <v>0.82733812949640284</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="45">
         <v>0.83812949640287771</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="44">
         <v>0.17266187050359713</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="45">
         <v>0.16187050359712229</v>
       </c>
       <c r="H29" s="4">
@@ -7209,7 +7330,7 @@
       <c r="V29" s="4"/>
       <c r="W29" s="5"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
@@ -7219,16 +7340,16 @@
       <c r="C30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="46">
         <v>0.8111510791366906</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="47">
         <v>0.84352517985611508</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="46">
         <v>0.18884892086330934</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="47">
         <v>0.15647482014388489</v>
       </c>
       <c r="H30" s="14">
@@ -7264,7 +7385,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="15"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>2</v>
       </c>
@@ -7274,19 +7395,27 @@
       <c r="C31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="18">
+      <c r="D31" s="41">
+        <v>0.98741007194244601</v>
+      </c>
+      <c r="E31" s="48">
         <v>0.98920863309352514</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18">
+      <c r="F31" s="41">
+        <v>1.2589928057553957E-2</v>
+      </c>
+      <c r="G31" s="48">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="H31" s="17"/>
+      <c r="H31" s="17">
+        <v>0.49683257918552037</v>
+      </c>
       <c r="I31" s="18">
         <v>0.49728752260397824</v>
       </c>
-      <c r="J31" s="17"/>
+      <c r="J31" s="17">
+        <v>0.98294215306487842</v>
+      </c>
       <c r="K31" s="18">
         <v>0.98384222097909368</v>
       </c>
@@ -7294,11 +7423,15 @@
       <c r="M31" s="18"/>
       <c r="N31" s="17"/>
       <c r="O31" s="18"/>
-      <c r="P31" s="17"/>
+      <c r="P31" s="17">
+        <v>0.49370503597122301</v>
+      </c>
       <c r="Q31" s="18">
         <v>0.49460431654676257</v>
       </c>
-      <c r="R31" s="17"/>
+      <c r="R31" s="17">
+        <v>0.97675456756896639</v>
+      </c>
       <c r="S31" s="18">
         <v>0.97853371978676051</v>
       </c>
@@ -7307,7 +7440,7 @@
       <c r="V31" s="17"/>
       <c r="W31" s="18"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -7317,16 +7450,16 @@
       <c r="C32" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="44">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="45">
         <v>0.98920863309352514</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="44">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="45">
         <v>1.0791366906474821E-2</v>
       </c>
       <c r="H32" s="4">
@@ -7362,7 +7495,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="5"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -7372,16 +7505,16 @@
       <c r="C33" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="44">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="45">
         <v>0.98561151079136688</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="44">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="45">
         <v>1.4388489208633094E-2</v>
       </c>
       <c r="H33" s="4">
@@ -7417,7 +7550,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="5"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>2</v>
       </c>
@@ -7427,16 +7560,16 @@
       <c r="C34" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="46">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="47">
         <v>0.99100719424460426</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="46">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="47">
         <v>8.9928057553956831E-3</v>
       </c>
       <c r="H34" s="14">
@@ -7472,7 +7605,7 @@
       <c r="V34" s="14"/>
       <c r="W34" s="15"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>2</v>
       </c>
@@ -7482,19 +7615,27 @@
       <c r="C35" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="18">
+      <c r="D35" s="41">
+        <v>0.98741007194244601</v>
+      </c>
+      <c r="E35" s="48">
         <v>0.98920863309352514</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18">
+      <c r="F35" s="41">
+        <v>1.2589928057553957E-2</v>
+      </c>
+      <c r="G35" s="48">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="H35" s="17"/>
+      <c r="H35" s="17">
+        <v>0.49683257918552037</v>
+      </c>
       <c r="I35" s="18">
         <v>0.49728752260397824</v>
       </c>
-      <c r="J35" s="17"/>
+      <c r="J35" s="17">
+        <v>0.98294215306487842</v>
+      </c>
       <c r="K35" s="18">
         <v>0.98384222097909368</v>
       </c>
@@ -7502,11 +7643,15 @@
       <c r="M35" s="18"/>
       <c r="N35" s="17"/>
       <c r="O35" s="18"/>
-      <c r="P35" s="17"/>
+      <c r="P35" s="17">
+        <v>0.49370503597122301</v>
+      </c>
       <c r="Q35" s="18">
         <v>0.49460431654676257</v>
       </c>
-      <c r="R35" s="17"/>
+      <c r="R35" s="17">
+        <v>0.97675456756896639</v>
+      </c>
       <c r="S35" s="18">
         <v>0.97853371978676051</v>
       </c>
@@ -7515,7 +7660,7 @@
       <c r="V35" s="17"/>
       <c r="W35" s="18"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -7525,16 +7670,16 @@
       <c r="C36" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="44">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="45">
         <v>0.98920863309352514</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="44">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="45">
         <v>1.0791366906474821E-2</v>
       </c>
       <c r="H36" s="4">
@@ -7570,7 +7715,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="5"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -7580,16 +7725,16 @@
       <c r="C37" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="44">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="45">
         <v>0.98561151079136688</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="44">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="45">
         <v>1.4388489208633094E-2</v>
       </c>
       <c r="H37" s="4">
@@ -7625,7 +7770,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="5"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>2</v>
       </c>
@@ -7635,16 +7780,16 @@
       <c r="C38" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="46">
         <v>0.98920863309352514</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="47">
         <v>0.99100719424460426</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="46">
         <v>1.0791366906474821E-2</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="47">
         <v>8.9928057553956831E-3</v>
       </c>
       <c r="H38" s="14">
@@ -7690,43 +7835,63 @@
       <c r="C39" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="17">
+        <v>0.78417266187050361</v>
+      </c>
       <c r="E39" s="18">
         <v>0.80215827338129497</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="17">
+        <v>7.1043165467625902E-2</v>
+      </c>
       <c r="G39" s="18">
         <v>7.4640287769784167E-2</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="17">
+        <v>0.62153862619029254</v>
+      </c>
       <c r="I39" s="18">
         <v>0.60817134474409873</v>
       </c>
-      <c r="J39" s="17"/>
+      <c r="J39" s="38">
+        <v>0.92427373914530475</v>
+      </c>
       <c r="K39" s="18">
         <v>0.91861313870512862</v>
       </c>
-      <c r="L39" s="17"/>
+      <c r="L39" s="17">
+        <v>0.2846514511566629</v>
+      </c>
       <c r="M39" s="18">
         <v>0.25956990985892719</v>
       </c>
-      <c r="N39" s="17"/>
+      <c r="N39" s="17">
+        <v>0.52941062502421821</v>
+      </c>
       <c r="O39" s="18">
         <v>0.47958183435062046</v>
       </c>
-      <c r="P39" s="17"/>
+      <c r="P39" s="17">
+        <v>0.56120503178429615</v>
+      </c>
       <c r="Q39" s="18">
         <v>0.54834565205649988</v>
       </c>
-      <c r="R39" s="17"/>
+      <c r="R39" s="17">
+        <v>0.88039056407206795</v>
+      </c>
       <c r="S39" s="18">
         <v>0.87413312317323055</v>
       </c>
-      <c r="T39" s="17"/>
+      <c r="T39" s="17">
+        <v>0.199545282303903</v>
+      </c>
       <c r="U39" s="18">
         <v>0.1767215900694547</v>
       </c>
-      <c r="V39" s="17"/>
+      <c r="V39" s="17">
+        <v>0.36993179234558543</v>
+      </c>
       <c r="W39" s="18">
         <v>0.32485314762819567</v>
       </c>
@@ -7824,7 +7989,7 @@
       <c r="G41" s="5">
         <v>7.1942446043165464E-2</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="37">
         <v>0.67368760520309157</v>
       </c>
       <c r="I41" s="5">
@@ -7886,13 +8051,13 @@
       <c r="D42" s="6">
         <v>0.7571942446043165</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="40">
         <v>0.81474820143884896</v>
       </c>
       <c r="F42" s="6">
         <v>8.363309352517985E-2</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="40">
         <v>6.9244604316546762E-2</v>
       </c>
       <c r="H42" s="6">
@@ -7944,7 +8109,7 @@
         <v>0.23429567325907405</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>3</v>
       </c>
@@ -7954,19 +8119,27 @@
       <c r="C43" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12">
+      <c r="D43" s="43">
+        <v>0.8794642857142857</v>
+      </c>
+      <c r="E43" s="42">
         <v>0.8616071428571429</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12">
+      <c r="F43" s="43">
+        <v>0.12053571428571429</v>
+      </c>
+      <c r="G43" s="42">
         <v>0.13839285714285715</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="11">
+        <v>0.68500000000000005</v>
+      </c>
       <c r="I43" s="12">
         <v>0.65703561021385881</v>
       </c>
-      <c r="J43" s="11"/>
+      <c r="J43" s="11">
+        <v>0.87062500000000009</v>
+      </c>
       <c r="K43" s="12">
         <v>0.85569467081542938</v>
       </c>
@@ -7974,11 +8147,15 @@
       <c r="M43" s="12"/>
       <c r="N43" s="11"/>
       <c r="O43" s="12"/>
-      <c r="P43" s="11"/>
+      <c r="P43" s="11">
+        <v>0.57676814988290404</v>
+      </c>
       <c r="Q43" s="12">
         <v>0.54952131297013906</v>
       </c>
-      <c r="R43" s="11"/>
+      <c r="R43" s="11">
+        <v>0.79934426229508193</v>
+      </c>
       <c r="S43" s="12">
         <v>0.77873546842945074</v>
       </c>
@@ -7987,7 +8164,7 @@
       <c r="V43" s="11"/>
       <c r="W43" s="12"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -7997,16 +8174,16 @@
       <c r="C44" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="44">
         <v>0.8772321428571429</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="45">
         <v>0.8325892857142857</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="44">
         <v>0.12276785714285714</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="45">
         <v>0.16741071428571427</v>
       </c>
       <c r="H44" s="4">
@@ -8042,7 +8219,7 @@
       <c r="V44" s="4"/>
       <c r="W44" s="5"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -8052,16 +8229,16 @@
       <c r="C45" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="44">
         <v>0.8861607142857143</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="45">
         <v>0.8928571428571429</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="44">
         <v>0.11383928571428571</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="45">
         <v>0.10714285714285714</v>
       </c>
       <c r="H45" s="4">
@@ -8097,7 +8274,7 @@
       <c r="V45" s="4"/>
       <c r="W45" s="5"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>3</v>
       </c>
@@ -8107,16 +8284,16 @@
       <c r="C46" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="46">
         <v>0.875</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="47">
         <v>0.8772321428571429</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="46">
         <v>0.125</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="47">
         <v>0.12276785714285714</v>
       </c>
       <c r="H46" s="14">
@@ -8152,7 +8329,7 @@
       <c r="V46" s="14"/>
       <c r="W46" s="15"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>3</v>
       </c>
@@ -8162,19 +8339,27 @@
       <c r="C47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18">
+      <c r="D47" s="41">
+        <v>0.8526785714285714</v>
+      </c>
+      <c r="E47" s="48">
         <v>0.8705357142857143</v>
       </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="18">
+      <c r="F47" s="41">
+        <v>0.14732142857142858</v>
+      </c>
+      <c r="G47" s="48">
         <v>0.12946428571428573</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="17">
+        <v>0.59239040529363107</v>
+      </c>
       <c r="I47" s="18">
         <v>0.61071492778809855</v>
       </c>
-      <c r="J47" s="17"/>
+      <c r="J47" s="17">
+        <v>0.83813733309701066</v>
+      </c>
       <c r="K47" s="18">
         <v>0.85065871422578743</v>
       </c>
@@ -8182,11 +8367,15 @@
       <c r="M47" s="18"/>
       <c r="N47" s="17"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="17"/>
+      <c r="P47" s="17">
+        <v>0.50123500352858152</v>
+      </c>
       <c r="Q47" s="18">
         <v>0.51920052424639584</v>
       </c>
-      <c r="R47" s="17"/>
+      <c r="R47" s="17">
+        <v>0.76332748386934157</v>
+      </c>
       <c r="S47" s="18">
         <v>0.78158204222055805</v>
       </c>
@@ -8195,7 +8384,7 @@
       <c r="V47" s="17"/>
       <c r="W47" s="18"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -8205,16 +8394,16 @@
       <c r="C48" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="44">
         <v>0.8772321428571429</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="45">
         <v>0.8504464285714286</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="44">
         <v>0.12276785714285714</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="45">
         <v>0.14955357142857142</v>
       </c>
       <c r="H48" s="4">
@@ -8250,7 +8439,7 @@
       <c r="V48" s="4"/>
       <c r="W48" s="5"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -8260,16 +8449,16 @@
       <c r="C49" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="44">
         <v>0.8616071428571429</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="45">
         <v>0.8861607142857143</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="44">
         <v>0.13839285714285715</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="45">
         <v>0.11383928571428571</v>
       </c>
       <c r="H49" s="4">
@@ -8305,7 +8494,7 @@
       <c r="V49" s="4"/>
       <c r="W49" s="5"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>3</v>
       </c>
@@ -8315,16 +8504,16 @@
       <c r="C50" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="46">
         <v>0.8794642857142857</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="47">
         <v>0.8727678571428571</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="46">
         <v>0.12053571428571429</v>
       </c>
-      <c r="G50" s="15">
+      <c r="G50" s="47">
         <v>0.12723214285714285</v>
       </c>
       <c r="H50" s="14">
@@ -8360,7 +8549,7 @@
       <c r="V50" s="14"/>
       <c r="W50" s="15"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>3</v>
       </c>
@@ -8370,19 +8559,27 @@
       <c r="C51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="18">
+      <c r="D51" s="41">
+        <v>0.8883928571428571</v>
+      </c>
+      <c r="E51" s="48">
         <v>0.8861607142857143</v>
       </c>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18">
+      <c r="F51" s="41">
+        <v>0.11160714285714286</v>
+      </c>
+      <c r="G51" s="48">
         <v>0.11383928571428571</v>
       </c>
-      <c r="H51" s="17"/>
+      <c r="H51" s="17">
+        <v>0.59109163928441033</v>
+      </c>
       <c r="I51" s="18">
         <v>0.6197007273756221</v>
       </c>
-      <c r="J51" s="17"/>
+      <c r="J51" s="17">
+        <v>0.86660114483909656</v>
+      </c>
       <c r="K51" s="18">
         <v>0.87123895501874915</v>
       </c>
@@ -8390,11 +8587,15 @@
       <c r="M51" s="18"/>
       <c r="N51" s="17"/>
       <c r="O51" s="18"/>
-      <c r="P51" s="17"/>
+      <c r="P51" s="17">
+        <v>0.51214733542319746</v>
+      </c>
       <c r="Q51" s="18">
         <v>0.53035727467335947</v>
       </c>
-      <c r="R51" s="17"/>
+      <c r="R51" s="17">
+        <v>0.80784503750559788</v>
+      </c>
       <c r="S51" s="18">
         <v>0.80924125597127461</v>
       </c>
@@ -8403,7 +8604,7 @@
       <c r="V51" s="17"/>
       <c r="W51" s="18"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -8413,16 +8614,16 @@
       <c r="C52" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="44">
         <v>0.8816964285714286</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="45">
         <v>0.875</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="44">
         <v>0.11830357142857142</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="45">
         <v>0.125</v>
       </c>
       <c r="H52" s="4">
@@ -8458,7 +8659,7 @@
       <c r="V52" s="4"/>
       <c r="W52" s="5"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -8468,16 +8669,16 @@
       <c r="C53" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="44">
         <v>0.8995535714285714</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="45">
         <v>0.8995535714285714</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="44">
         <v>0.10044642857142858</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="45">
         <v>0.10044642857142858</v>
       </c>
       <c r="H53" s="4">
@@ -8513,7 +8714,7 @@
       <c r="V53" s="4"/>
       <c r="W53" s="5"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>3</v>
       </c>
@@ -8523,16 +8724,16 @@
       <c r="C54" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="46">
         <v>0.8950892857142857</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="47">
         <v>0.890625</v>
       </c>
-      <c r="F54" s="14">
+      <c r="F54" s="46">
         <v>0.10491071428571429</v>
       </c>
-      <c r="G54" s="15">
+      <c r="G54" s="47">
         <v>0.109375</v>
       </c>
       <c r="H54" s="14">
@@ -8578,43 +8779,63 @@
       <c r="C55" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="17"/>
+      <c r="D55" s="17">
+        <v>0.7544642857142857</v>
+      </c>
       <c r="E55" s="18">
         <v>0.7745535714285714</v>
       </c>
-      <c r="F55" s="17"/>
+      <c r="F55" s="17">
+        <v>0.12648809523809523</v>
+      </c>
       <c r="G55" s="18">
         <v>0.12723214285714285</v>
       </c>
-      <c r="H55" s="17"/>
+      <c r="H55" s="17">
+        <v>0.62282734819268049</v>
+      </c>
       <c r="I55" s="18">
         <v>0.62915042179252645</v>
       </c>
-      <c r="J55" s="17"/>
-      <c r="K55" s="18">
+      <c r="J55" s="17">
+        <v>0.8584544926453691</v>
+      </c>
+      <c r="K55" s="48">
         <v>0.85919744668665532</v>
       </c>
-      <c r="L55" s="17"/>
+      <c r="L55" s="17">
+        <v>0.31553030303030305</v>
+      </c>
       <c r="M55" s="18">
         <v>0.32873655086268833</v>
       </c>
-      <c r="N55" s="17"/>
+      <c r="N55" s="17">
+        <v>0.32000383582662068</v>
+      </c>
       <c r="O55" s="18">
         <v>0.33052360032265243</v>
       </c>
-      <c r="P55" s="17"/>
+      <c r="P55" s="17">
+        <v>0.53005016294489427</v>
+      </c>
       <c r="Q55" s="18">
         <v>0.53302637062996483</v>
       </c>
-      <c r="R55" s="17"/>
+      <c r="R55" s="17">
+        <v>0.7901722612233405</v>
+      </c>
       <c r="S55" s="18">
         <v>0.78985292220709447</v>
       </c>
-      <c r="T55" s="17"/>
+      <c r="T55" s="17">
+        <v>0.19059239610963749</v>
+      </c>
       <c r="U55" s="18">
         <v>0.19758345509722378</v>
       </c>
-      <c r="V55" s="17"/>
+      <c r="V55" s="17">
+        <v>0.19382466507739315</v>
+      </c>
       <c r="W55" s="18">
         <v>0.19889758032504201</v>
       </c>
@@ -8703,25 +8924,25 @@
       <c r="D57" s="4">
         <v>0.7723214285714286</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="39">
         <v>0.8169642857142857</v>
       </c>
       <c r="F57" s="4">
         <v>0.11755952380952381</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="39">
         <v>0.10714285714285714</v>
       </c>
       <c r="H57" s="4">
         <v>0.60714629621656435</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I57" s="39">
         <v>0.63647963598478885</v>
       </c>
       <c r="J57" s="4">
         <v>0.85898122847531033</v>
       </c>
-      <c r="K57" s="5">
+      <c r="K57" s="39">
         <v>0.87016704731159988</v>
       </c>
       <c r="L57" s="4">
@@ -8832,7 +9053,7 @@
         <v>3.5980291338990451E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
@@ -8842,19 +9063,27 @@
       <c r="C59" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="12">
+      <c r="D59" s="43">
+        <v>0.87128712871287128</v>
+      </c>
+      <c r="E59" s="42">
         <v>0.8571428571428571</v>
       </c>
-      <c r="F59" s="11"/>
-      <c r="G59" s="12">
+      <c r="F59" s="43">
+        <v>0.12871287128712872</v>
+      </c>
+      <c r="G59" s="42">
         <v>0.14285714285714285</v>
       </c>
-      <c r="H59" s="11"/>
+      <c r="H59" s="11">
+        <v>0.70033023899242175</v>
+      </c>
       <c r="I59" s="12">
         <v>0.6460321315798605</v>
       </c>
-      <c r="J59" s="11"/>
+      <c r="J59" s="11">
+        <v>0.86136266507741444</v>
+      </c>
       <c r="K59" s="12">
         <v>0.84051692088056984</v>
       </c>
@@ -8862,11 +9091,15 @@
       <c r="M59" s="12"/>
       <c r="N59" s="11"/>
       <c r="O59" s="12"/>
-      <c r="P59" s="11"/>
+      <c r="P59" s="11">
+        <v>0.58698471198471203</v>
+      </c>
       <c r="Q59" s="12">
         <v>0.53991002063436577</v>
       </c>
-      <c r="R59" s="11"/>
+      <c r="R59" s="11">
+        <v>0.7836161994577836</v>
+      </c>
       <c r="S59" s="12">
         <v>0.76110365668023505</v>
       </c>
@@ -8875,7 +9108,7 @@
       <c r="V59" s="11"/>
       <c r="W59" s="12"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -8885,16 +9118,16 @@
       <c r="C60" t="s">
         <v>18</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="44">
         <v>0.85431400282885428</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="45">
         <v>0.85007072135785011</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="44">
         <v>0.14568599717114569</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="45">
         <v>0.14992927864214992</v>
       </c>
       <c r="H60" s="4">
@@ -8930,7 +9163,7 @@
       <c r="V60" s="4"/>
       <c r="W60" s="5"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -8940,16 +9173,16 @@
       <c r="C61" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="44">
         <v>0.85572842998585574</v>
       </c>
-      <c r="E61" s="5">
+      <c r="E61" s="45">
         <v>0.86987270155586982</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="44">
         <v>0.14427157001414428</v>
       </c>
-      <c r="G61" s="5">
+      <c r="G61" s="45">
         <v>0.13012729844413012</v>
       </c>
       <c r="H61" s="4">
@@ -8985,7 +9218,7 @@
       <c r="V61" s="4"/>
       <c r="W61" s="5"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>4</v>
       </c>
@@ -8995,16 +9228,16 @@
       <c r="C62" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="14">
+      <c r="D62" s="46">
         <v>0.85997171145686002</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="47">
         <v>0.85855728429985856</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="46">
         <v>0.14002828854314003</v>
       </c>
-      <c r="G62" s="15">
+      <c r="G62" s="47">
         <v>0.14144271570014144</v>
       </c>
       <c r="H62" s="14">
@@ -9040,7 +9273,7 @@
       <c r="V62" s="14"/>
       <c r="W62" s="15"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>4</v>
       </c>
@@ -9050,19 +9283,27 @@
       <c r="C63" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="18">
+      <c r="D63" s="41">
+        <v>0.942008486562942</v>
+      </c>
+      <c r="E63" s="48">
         <v>0.94059405940594054</v>
       </c>
-      <c r="F63" s="17"/>
-      <c r="G63" s="18">
+      <c r="F63" s="41">
+        <v>5.7991513437057989E-2</v>
+      </c>
+      <c r="G63" s="48">
         <v>5.9405940594059403E-2</v>
       </c>
-      <c r="H63" s="17"/>
+      <c r="H63" s="17">
+        <v>0.6694189428066375</v>
+      </c>
       <c r="I63" s="18">
         <v>0.65631944444444446</v>
       </c>
-      <c r="J63" s="17"/>
+      <c r="J63" s="17">
+        <v>0.93139362894003297</v>
+      </c>
       <c r="K63" s="18">
         <v>0.92909928492849281</v>
       </c>
@@ -9070,11 +9311,15 @@
       <c r="M63" s="18"/>
       <c r="N63" s="17"/>
       <c r="O63" s="18"/>
-      <c r="P63" s="17"/>
+      <c r="P63" s="17">
+        <v>0.58371114429211346</v>
+      </c>
       <c r="Q63" s="18">
         <v>0.57360117111255693</v>
       </c>
-      <c r="R63" s="17"/>
+      <c r="R63" s="17">
+        <v>0.89552396299181192</v>
+      </c>
       <c r="S63" s="18">
         <v>0.89305706758053816</v>
       </c>
@@ -9083,7 +9328,7 @@
       <c r="V63" s="17"/>
       <c r="W63" s="18"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -9093,16 +9338,16 @@
       <c r="C64" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="44">
         <v>0.93493635077793491</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="45">
         <v>0.93210749646393209</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="44">
         <v>6.5063649222065062E-2</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G64" s="45">
         <v>6.7892503536067891E-2</v>
       </c>
       <c r="H64" s="4">
@@ -9138,7 +9383,7 @@
       <c r="V64" s="4"/>
       <c r="W64" s="5"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -9148,16 +9393,16 @@
       <c r="C65" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D65" s="44">
         <v>0.92927864214992928</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="45">
         <v>0.93917963224893919</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65" s="44">
         <v>7.0721357850070721E-2</v>
       </c>
-      <c r="G65" s="5">
+      <c r="G65" s="45">
         <v>6.0820367751060818E-2</v>
       </c>
       <c r="H65" s="4">
@@ -9193,7 +9438,7 @@
       <c r="V65" s="4"/>
       <c r="W65" s="5"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>4</v>
       </c>
@@ -9203,16 +9448,16 @@
       <c r="C66" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="14">
+      <c r="D66" s="46">
         <v>0.93635077793493637</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="47">
         <v>0.93917963224893919</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F66" s="46">
         <v>6.3649222065063654E-2</v>
       </c>
-      <c r="G66" s="15">
+      <c r="G66" s="47">
         <v>6.0820367751060818E-2</v>
       </c>
       <c r="H66" s="14">
@@ -9258,43 +9503,63 @@
       <c r="C67" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D67" s="17"/>
+      <c r="D67" s="38">
+        <v>0.75813295615275811</v>
+      </c>
       <c r="E67" s="18">
         <v>0.74398868458274403</v>
       </c>
-      <c r="F67" s="17"/>
+      <c r="F67" s="38">
+        <v>9.2409240924092403E-2</v>
+      </c>
       <c r="G67" s="18">
         <v>0.10466760961810467</v>
       </c>
-      <c r="H67" s="17"/>
+      <c r="H67" s="38">
+        <v>0.7429181804634114</v>
+      </c>
       <c r="I67" s="18">
         <v>0.70483835356124869</v>
       </c>
-      <c r="J67" s="17"/>
+      <c r="J67" s="38">
+        <v>0.90074431865645233</v>
+      </c>
       <c r="K67" s="18">
         <v>0.88443688473656801</v>
       </c>
-      <c r="L67" s="17"/>
+      <c r="L67" s="17">
+        <v>0.53928903195369038</v>
+      </c>
       <c r="M67" s="18">
         <v>0.46967593711482225</v>
       </c>
-      <c r="N67" s="17"/>
+      <c r="N67" s="17">
+        <v>0.60540555510253691</v>
+      </c>
       <c r="O67" s="18">
         <v>0.52536805160130673</v>
       </c>
-      <c r="P67" s="17"/>
+      <c r="P67" s="17">
+        <v>0.64439549008877106</v>
+      </c>
       <c r="Q67" s="18">
         <v>0.60482542884089907</v>
       </c>
-      <c r="R67" s="17"/>
+      <c r="R67" s="17">
+        <v>0.83986454293094626</v>
+      </c>
       <c r="S67" s="18">
         <v>0.81918571590509481</v>
       </c>
-      <c r="T67" s="17"/>
+      <c r="T67" s="17">
+        <v>0.38973502099722007</v>
+      </c>
       <c r="U67" s="18">
         <v>0.32210556938700391</v>
       </c>
-      <c r="V67" s="17"/>
+      <c r="V67" s="17">
+        <v>0.45550384902986135</v>
+      </c>
       <c r="W67" s="18">
         <v>0.37344149392267861</v>
       </c>
@@ -9512,7 +9777,7 @@
         <v>0.23807755407834749</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>4</v>
       </c>
@@ -9522,19 +9787,27 @@
       <c r="C71" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D71" s="17"/>
-      <c r="E71" s="18">
+      <c r="D71" s="41">
+        <v>0.90947666195190946</v>
+      </c>
+      <c r="E71" s="48">
         <v>0.88826025459688829</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="18">
+      <c r="F71" s="41">
+        <v>9.0523338048090526E-2</v>
+      </c>
+      <c r="G71" s="48">
         <v>0.11173974540311174</v>
       </c>
-      <c r="H71" s="17"/>
+      <c r="H71" s="17">
+        <v>0.8590053595911753</v>
+      </c>
       <c r="I71" s="18">
         <v>0.81216348465944066</v>
       </c>
-      <c r="J71" s="17"/>
+      <c r="J71" s="17">
+        <v>0.90947666195190946</v>
+      </c>
       <c r="K71" s="18">
         <v>0.88369444840064137</v>
       </c>
@@ -9542,11 +9815,15 @@
       <c r="M71" s="18"/>
       <c r="N71" s="17"/>
       <c r="O71" s="18"/>
-      <c r="P71" s="17"/>
+      <c r="P71" s="17">
+        <v>0.7624906139894877</v>
+      </c>
       <c r="Q71" s="18">
         <v>0.7009650947757744</v>
       </c>
-      <c r="R71" s="17"/>
+      <c r="R71" s="17">
+        <v>0.84045346634324314</v>
+      </c>
       <c r="S71" s="18">
         <v>0.80339642345451112</v>
       </c>
@@ -9555,7 +9832,7 @@
       <c r="V71" s="17"/>
       <c r="W71" s="18"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -9565,16 +9842,16 @@
       <c r="C72" t="s">
         <v>18</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D72" s="44">
         <v>0.82885431400282883</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="45">
         <v>0.80622347949080619</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="44">
         <v>0.17114568599717114</v>
       </c>
-      <c r="G72" s="5">
+      <c r="G72" s="45">
         <v>0.19377652050919378</v>
       </c>
       <c r="H72" s="4">
@@ -9610,7 +9887,7 @@
       <c r="V72" s="4"/>
       <c r="W72" s="5"/>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -9620,16 +9897,16 @@
       <c r="C73" t="s">
         <v>19</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="44">
         <v>0.89533239038189538</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="45">
         <v>0.89250353606789246</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="44">
         <v>0.10466760961810467</v>
       </c>
-      <c r="G73" s="5">
+      <c r="G73" s="45">
         <v>0.1074964639321075</v>
       </c>
       <c r="H73" s="4">
@@ -9665,7 +9942,7 @@
       <c r="V73" s="4"/>
       <c r="W73" s="5"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>4</v>
       </c>
@@ -9675,16 +9952,16 @@
       <c r="C74" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="49">
         <v>0.87694483734087691</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="50">
         <v>0.85572842998585574</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74" s="49">
         <v>0.12305516265912306</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="50">
         <v>0.14427157001414428</v>
       </c>
       <c r="H74" s="6">
@@ -9726,94 +10003,94 @@
       </c>
       <c r="D76" s="2" cm="1">
         <f t="array" ref="D76">COUNT(IF(D3:D74&gt;E3:E74,1))</f>
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E76" s="3" cm="1">
         <f t="array" ref="E76">COUNT(IF(E3:E74&gt;D3:D74,1))</f>
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F76" s="2" cm="1">
         <f t="array" ref="F76">COUNT(IF(F3:F74&lt;G3:G74,1))</f>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G76" s="3" cm="1">
         <f t="array" ref="G76">COUNT(IF(G3:G74&lt;F3:F74,1))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H76" s="2" cm="1">
         <f t="array" ref="H76">COUNT(IF(H3:H74&gt;I3:I74,1))</f>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I76" s="3" cm="1">
         <f t="array" ref="I76">COUNT(IF(I3:I74&gt;H3:H74,1))</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J76" s="2" cm="1">
         <f t="array" ref="J76">COUNT(IF(J3:J74&gt;K3:K74,1))</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="K76" s="3" cm="1">
         <f t="array" ref="K76">COUNT(IF(K3:K74&gt;J3:J74,1))</f>
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L76" s="2" cm="1">
         <f t="array" ref="L76">COUNT(IF(L3:L74&gt;M3:M74,1))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M76" s="3" cm="1">
         <f t="array" ref="M76">COUNT(IF(M3:M74&gt;L3:L74,1))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N76" s="2" cm="1">
         <f t="array" ref="N76">COUNT(IF(N3:N74&gt;O3:O74,1))</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O76" s="3" cm="1">
         <f t="array" ref="O76">COUNT(IF(O3:O74&gt;N3:N74,1))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P76" s="2" cm="1">
         <f t="array" ref="P76">COUNT(IF(P3:P74&gt;Q3:Q74,1))</f>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="Q76" s="3" cm="1">
         <f t="array" ref="Q76">COUNT(IF(Q3:Q74&gt;P3:P74,1))</f>
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="R76" s="2" cm="1">
         <f t="array" ref="R76">COUNT(IF(R3:R74&gt;S3:S74,1))</f>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S76" s="3" cm="1">
         <f t="array" ref="S76">COUNT(IF(S3:S74&gt;R3:R74,1))</f>
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="T76" s="2" cm="1">
         <f t="array" ref="T76">COUNT(IF(T3:T74&gt;U3:U74,1))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U76" s="3" cm="1">
         <f t="array" ref="U76">COUNT(IF(U3:U74&gt;T3:T74,1))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V76" s="2" cm="1">
         <f t="array" ref="V76">COUNT(IF(V3:V74&gt;W3:W74,1))</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="W76" s="3" cm="1">
         <f t="array" ref="W76">COUNT(IF(W3:W74&gt;V3:V74,1))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:C74" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Overall"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="13">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -9821,6 +10098,12 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D74">
     <cfRule type="expression" dxfId="19" priority="20">
@@ -9928,6 +10211,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007BDDFC7A116ECA4DBFB88BC5780DB34C" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c8e8c60cc40489f3ad8701c5ba8dfe2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="014ef4ca-692b-4eb1-8e39-c3c634a1a31a" xmlns:ns3="d5396ee2-9d20-4c1e-9b02-c7d8815090c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6b790f8f3849a01e14db75be7a5dd92" ns2:_="" ns3:_="">
     <xsd:import namespace="014ef4ca-692b-4eb1-8e39-c3c634a1a31a"/>
@@ -10156,16 +10448,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5A5817-A92D-4A00-9695-56D13E6EE86B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F032BF8A-4D03-4BF9-B5AC-BCF6B4ED4F80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10182,12 +10473,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5A5817-A92D-4A00-9695-56D13E6EE86B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>